<commit_message>
Adding some updated results for full graph analysis
</commit_message>
<xml_diff>
--- a/Results/Full_Graph_Results.xlsx
+++ b/Results/Full_Graph_Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Subreddit</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>funny</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>FULL_GRAPHS</t>
   </si>
 </sst>
 </file>
@@ -444,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +463,7 @@
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
     <col min="9" max="10" width="23.28515625" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" customWidth="1"/>
@@ -467,163 +473,86 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>81944</v>
-      </c>
-      <c r="C2">
-        <v>599081</v>
-      </c>
-      <c r="D2">
-        <v>7.3109999999999999</v>
-      </c>
-      <c r="E2">
-        <v>11.725</v>
-      </c>
-      <c r="F2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="G2">
-        <v>235</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2">
-        <v>0.35199999999999998</v>
-      </c>
-      <c r="L2">
-        <v>281</v>
-      </c>
-      <c r="M2">
-        <v>0.26630315551046901</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>211824</v>
-      </c>
-      <c r="C3">
-        <v>681715</v>
-      </c>
-      <c r="D3">
-        <v>3.218</v>
-      </c>
-      <c r="E3">
-        <v>3.9660000000000002</v>
-      </c>
-      <c r="F3">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="G3">
-        <v>11020</v>
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3">
-        <v>0.53</v>
-      </c>
-      <c r="L3">
-        <v>11032</v>
-      </c>
-      <c r="M3">
-        <v>0.94084624512705095</v>
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>31191</v>
+        <v>81944</v>
       </c>
       <c r="C4">
-        <v>71941</v>
+        <v>599081</v>
       </c>
       <c r="D4">
-        <v>2.306</v>
+        <v>7.3109999999999999</v>
       </c>
       <c r="E4">
-        <v>2.4809999999999999</v>
+        <v>11.725</v>
       </c>
       <c r="F4">
-        <v>1.7000000000000001E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="G4">
-        <v>1286</v>
-      </c>
-      <c r="H4">
-        <v>19107</v>
-      </c>
-      <c r="I4">
-        <v>6.133</v>
-      </c>
-      <c r="J4">
-        <v>20</v>
+        <v>235</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
       </c>
       <c r="K4">
-        <v>0.52500000000000002</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="L4">
-        <v>1347</v>
+        <v>281</v>
       </c>
       <c r="M4">
         <v>0.26630315551046901</v>
@@ -631,224 +560,330 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>7019</v>
+        <v>211824</v>
       </c>
       <c r="C5">
-        <v>20223</v>
+        <v>681715</v>
       </c>
       <c r="D5">
-        <v>2.8809999999999998</v>
+        <v>3.218</v>
       </c>
       <c r="E5">
-        <v>3.5139999999999998</v>
+        <v>3.9660000000000002</v>
       </c>
       <c r="F5">
-        <v>3.6999999999999998E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G5">
-        <v>192</v>
-      </c>
-      <c r="H5">
-        <v>3518</v>
-      </c>
-      <c r="I5">
-        <v>5.0599999999999996</v>
-      </c>
-      <c r="J5">
-        <v>14</v>
+        <v>11020</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
       </c>
       <c r="K5">
-        <v>0.51300000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="L5">
-        <v>219</v>
+        <v>11032</v>
       </c>
       <c r="M5">
-        <v>0.15974870601938301</v>
+        <v>0.94084624512705095</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>107176</v>
+        <v>31191</v>
       </c>
       <c r="C6">
-        <v>596201</v>
+        <v>71941</v>
       </c>
       <c r="D6">
-        <v>5.5629999999999997</v>
+        <v>2.306</v>
       </c>
       <c r="E6">
-        <v>6.0039999999999996</v>
+        <v>2.4809999999999999</v>
       </c>
       <c r="F6">
-        <v>2.1999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G6">
-        <v>1685</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
+        <v>1286</v>
+      </c>
+      <c r="H6">
+        <v>19107</v>
+      </c>
+      <c r="I6">
+        <v>6.133</v>
+      </c>
+      <c r="J6">
+        <v>20</v>
       </c>
       <c r="K6">
-        <v>0.34</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="L6">
-        <v>1938</v>
+        <v>1347</v>
       </c>
       <c r="M6">
-        <v>0.31415906756739098</v>
+        <v>0.26630315551046901</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>7991</v>
+        <v>7019</v>
       </c>
       <c r="C7">
-        <v>29616</v>
+        <v>20223</v>
       </c>
       <c r="D7">
-        <v>3.706</v>
+        <v>2.8809999999999998</v>
       </c>
       <c r="E7">
-        <v>4.6520000000000001</v>
+        <v>3.5139999999999998</v>
       </c>
       <c r="F7">
-        <v>4.9000000000000002E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="G7">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="H7">
-        <v>3269</v>
+        <v>3518</v>
       </c>
       <c r="I7">
-        <v>4.66371824173972</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="J7">
         <v>14</v>
       </c>
       <c r="K7">
-        <v>0.5</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="L7">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="M7">
-        <v>0.10767787663865599</v>
+        <v>0.15974870601938301</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>3776</v>
+        <v>107176</v>
       </c>
       <c r="C8">
-        <v>14720</v>
+        <v>596201</v>
       </c>
       <c r="D8">
-        <v>3.8980000000000001</v>
+        <v>5.5629999999999997</v>
       </c>
       <c r="E8">
-        <v>22.082000000000001</v>
+        <v>6.0039999999999996</v>
       </c>
       <c r="F8">
-        <v>6.5000000000000002E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G8">
-        <v>167</v>
-      </c>
-      <c r="H8">
-        <v>1546</v>
-      </c>
-      <c r="I8">
-        <v>4.3776075547582298</v>
-      </c>
-      <c r="J8">
-        <v>13</v>
+        <v>1685</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
       </c>
       <c r="K8">
-        <v>0.46600000000000003</v>
+        <v>0.34</v>
       </c>
       <c r="L8">
-        <v>181</v>
+        <v>1938</v>
       </c>
       <c r="M8">
-        <v>6.7556107230851495E-2</v>
+        <v>0.31415906756739098</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9">
-        <v>100084</v>
+        <v>7991</v>
       </c>
       <c r="C9">
-        <v>219535</v>
+        <v>29616</v>
       </c>
       <c r="D9">
-        <v>2.194</v>
+        <v>3.706</v>
       </c>
       <c r="E9">
-        <v>3.3370000000000002</v>
+        <v>4.6520000000000001</v>
       </c>
       <c r="F9">
-        <v>3.5000000000000003E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="G9">
-        <v>6425</v>
+        <v>168</v>
       </c>
       <c r="H9">
-        <v>53486</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" t="s">
-        <v>18</v>
+        <v>3269</v>
+      </c>
+      <c r="I9">
+        <v>4.66371824173972</v>
+      </c>
+      <c r="J9">
+        <v>14</v>
       </c>
       <c r="K9">
-        <v>0.71199999999999997</v>
+        <v>0.5</v>
       </c>
       <c r="L9">
-        <v>6475</v>
+        <v>182</v>
       </c>
       <c r="M9">
-        <v>0.66405480069118294</v>
+        <v>0.10767787663865599</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>3776</v>
+      </c>
+      <c r="C10">
+        <v>14720</v>
+      </c>
+      <c r="D10">
+        <v>3.8980000000000001</v>
+      </c>
+      <c r="E10">
+        <v>22.082000000000001</v>
+      </c>
+      <c r="F10">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G10">
+        <v>167</v>
+      </c>
+      <c r="H10">
+        <v>1546</v>
+      </c>
+      <c r="I10">
+        <v>4.3776075547582298</v>
+      </c>
+      <c r="J10">
+        <v>13</v>
+      </c>
+      <c r="K10">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="L10">
+        <v>181</v>
+      </c>
+      <c r="M10">
+        <v>6.7556107230851495E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>100084</v>
+      </c>
+      <c r="C11">
+        <v>219535</v>
+      </c>
+      <c r="D11">
+        <v>2.194</v>
+      </c>
+      <c r="E11">
+        <v>3.3370000000000002</v>
+      </c>
+      <c r="F11">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G11">
+        <v>6425</v>
+      </c>
+      <c r="H11">
+        <v>53486</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="L11">
+        <v>6475</v>
+      </c>
+      <c r="M11">
+        <v>0.66405480069118294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <v>2081060</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <v>6800098</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>3.2679999999999998</v>
       </c>
-      <c r="E10">
+      <c r="E12">
         <v>3.3959999999999999</v>
+      </c>
+      <c r="F12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12">
+        <v>3.2274247996377299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>